<commit_message>
added reshenie_shablon and fixed bugs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\tabl-todocx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fd\tabl-to-docx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B779CC1-BEB0-4CAA-89E5-960ABBB00311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBE842D-872D-45C9-92D6-D26CDA1B94EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="4320" windowWidth="21600" windowHeight="11385" xr2:uid="{B2319DB0-4B47-40B6-AF53-D929A68305A6}"/>
+    <workbookView xWindow="4350" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{B2319DB0-4B47-40B6-AF53-D929A68305A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ФИО</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>подпись</t>
+  </si>
+  <si>
+    <t>Дата для решения</t>
   </si>
 </sst>
 </file>
@@ -101,9 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -419,38 +423,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393F02A2-ABA9-48C6-880E-83C853752E96}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -468,38 +473,12 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>